<commit_message>
edited the repeater method to proccess the 4 bio stocks
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/Repeater/HZNP/HZNPBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/Repeater/HZNP/HZNPBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -436,21 +436,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y31"/>
+  <dimension ref="A1:Y32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -2833,6 +2833,83 @@
       <c r="W31">
         <v>0</v>
       </c>
+      <c r="X31">
+        <v>-0.21000000000000085</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>42651.425162037034</v>
+      </c>
+      <c r="B32">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32">
+        <v>56</v>
+      </c>
+      <c r="E32">
+        <v>1623</v>
+      </c>
+      <c r="F32">
+        <v>181</v>
+      </c>
+      <c r="G32">
+        <v>69</v>
+      </c>
+      <c r="H32">
+        <v>30</v>
+      </c>
+      <c r="I32">
+        <v>94</v>
+      </c>
+      <c r="J32">
+        <v>5</v>
+      </c>
+      <c r="K32">
+        <v>4610</v>
+      </c>
+      <c r="L32">
+        <v>23</v>
+      </c>
+      <c r="M32">
+        <v>10</v>
+      </c>
+      <c r="N32">
+        <v>16</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q32">
+        <v>47.963765586266284</v>
+      </c>
+      <c r="R32">
+        <v>0.49</v>
+      </c>
+      <c r="S32" s="2">
+        <v>5.21E-2</v>
+      </c>
+      <c r="T32" s="2">
+        <v>-2.1399999999999999E-2</v>
+      </c>
+      <c r="U32">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="V32" t="s">
+        <v>27</v>
+      </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>